<commit_message>
se agrego todo lo de tips
</commit_message>
<xml_diff>
--- a/m4u2/public/img/base datos.xlsx
+++ b/m4u2/public/img/base datos.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4368fbe0d7469ba/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4368fbe0d7469ba/Desktop/diplomatura-lopardo/m4u2/public/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_AD4D2F04E46CFB4ACB3E20EA55D0F206683EDF15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E2428B5-D6EA-41F2-831B-1C6842BC4DF4}"/>
+  <xr:revisionPtr revIDLastSave="237" documentId="11_AD4D2F04E46CFB4ACB3E20EA55D0F206683EDF15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2212FB2D-303E-47C7-B7B1-A01AF3F0021E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="destinos" sheetId="1" r:id="rId1"/>
+    <sheet name="tips" sheetId="2" r:id="rId2"/>
+    <sheet name="iconos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="112">
   <si>
     <t>nombre</t>
   </si>
@@ -199,6 +201,185 @@
   </si>
   <si>
     <t>tango-porteño.jpg</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>subtitulo</t>
+  </si>
+  <si>
+    <t>icono_id</t>
+  </si>
+  <si>
+    <t>clase</t>
+  </si>
+  <si>
+    <t>Reciclaje</t>
+  </si>
+  <si>
+    <t>fa-solid fa-recycle</t>
+  </si>
+  <si>
+    <t>Naturaleza</t>
+  </si>
+  <si>
+    <t>fa-solid fa-seedling</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>fa-solid fa-mobile-screen</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>fa-solid fa-bus</t>
+  </si>
+  <si>
+    <t>Residuos</t>
+  </si>
+  <si>
+    <t>fa-solid fa-trash-can-arrow-up</t>
+  </si>
+  <si>
+    <t>Energía</t>
+  </si>
+  <si>
+    <t>fa-regular fa-lightbulb</t>
+  </si>
+  <si>
+    <t>Mapa</t>
+  </si>
+  <si>
+    <t>fa-solid fa-map</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>fa-solid fa-hotel</t>
+  </si>
+  <si>
+    <t>Transporte Público</t>
+  </si>
+  <si>
+    <t>¡Tu huella también cuenta!</t>
+  </si>
+  <si>
+    <t>Al elegir transporte público, como colectivos, subtes o trenes, en vez de vehículos particulares, reducís significativamente tus emisiones de carbono.
+Planificar tu viaje con conciencia ambiental también es parte del compromiso con el planeta.</t>
+  </si>
+  <si>
+    <t>Llevá siempre contigo una botella de agua reutilizable, un termo para el café y bolsas de tela. Cada acción suma para evitar el uso de plásticos.
+Si no podés evitar el plástico, trata de reciclarlo o llevarlo a puntos de recolección selectiva.</t>
+  </si>
+  <si>
+    <t>Optá por productos reutilizables.</t>
+  </si>
+  <si>
+    <t>Movilidad Activa</t>
+  </si>
+  <si>
+    <t>Bicicleta</t>
+  </si>
+  <si>
+    <t>fa-solid fa-person-biking</t>
+  </si>
+  <si>
+    <t>fa-solid fa-person-walking</t>
+  </si>
+  <si>
+    <t>Caminata</t>
+  </si>
+  <si>
+    <t>¡Usá la bici y recorre la ciudad!</t>
+  </si>
+  <si>
+    <t>Camina o usa bicicleta para distancias cortas.
+La Ciudad de Buenos Aires tiene un sistema de bicicletas públicas gratuitas llamado EcoBici, que te permite recorrer el centro y otras zonas de forma gratuita.
+¡Solo necesitás registrarte en la app y comenzar a pedalear!</t>
+  </si>
+  <si>
+    <t>Llevá pasajes, reservas y documentos en el celular en lugar de imprimirlos.
+Hoy en día la mayoría de aerolíneas, hoteles y transportes aceptan comprobantes digitales. Además de ahorrar papel, evitás perder documentación durante el viaje.</t>
+  </si>
+  <si>
+    <t>Documentación Digital</t>
+  </si>
+  <si>
+    <t>Llevá siempre una botella reutilizable y evitá comprar botellas descartables.
+En muchas zonas de Buenos Aires podés recargar agua potable en bares, estaciones y espacios públicos.
+Además de cuidarte, ayudás a reducir el consumo de plástico y el gasto innecesario de agua.</t>
+  </si>
+  <si>
+    <t>Tomá agua sin desperdiciar</t>
+  </si>
+  <si>
+    <t>Hidratación consciente</t>
+  </si>
+  <si>
+    <t>Compra en mercados locales y apoya proyectos comunitarios sustentables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Apoya lo Local</t>
+  </si>
+  <si>
+    <t>Cuidado con el consumo masivo</t>
+  </si>
+  <si>
+    <t>Evitá comprar productos descartables o souvenirs de uso innecesario.
+Priorizar calidad sobre cantidad reduce residuos y el impacto ambiental del turismo masivo.
+Elegir con conciencia también es una forma de cuidar el planeta.</t>
+  </si>
+  <si>
+    <t>Comprá solo lo necesario.</t>
+  </si>
+  <si>
+    <t>No dejes residuos, respetá la flora y la fauna y mantenete en los senderos habilitados.
+Cuidar los espacios naturales permite que más personas puedan disfrutarlos hoy y en el futuro.
+Viajar también es aprender a convivir con el entorno.</t>
+  </si>
+  <si>
+    <t>Respetá cada lugar que visitás</t>
+  </si>
+  <si>
+    <t>Respetá la naturaleza</t>
+  </si>
+  <si>
+    <t>Cuida el Agua</t>
+  </si>
+  <si>
+    <t>Menos desperdicio de agua</t>
+  </si>
+  <si>
+    <t>Evitá dejar correr el agua innecesariamente y cerrá bien las canillas luego de usarlas.
+Pequeñas acciones, como no desperdiciar agua al lavar objetos o manos,ayudan a conservar uno de los recursos más importantes del planeta.</t>
+  </si>
+  <si>
+    <t>Separá residuos siempre que sea posible y evitá tirar basura en espacios públicos.
+Muchos destinos cuentan con puntos de reciclaje que ayudan a reducir el impacto ambiental.
+Cada residuo bien gestionado suma.</t>
+  </si>
+  <si>
+    <t>¡Reducí, reutilizá y recicla!</t>
+  </si>
+  <si>
+    <t>Gestioná tus residuos</t>
+  </si>
+  <si>
+    <t>Ahorrá energía</t>
+  </si>
+  <si>
+    <t>Pequeñas acciones, gran impacto</t>
+  </si>
+  <si>
+    <t>Apagá luces, aire acondicionado y dispositivos cuando no los estés usando.
+Reducir el consumo de energía ayuda a disminuir las emisiones y el gasto innecesario de recursos.
+Ser responsable también es parte del viaje.</t>
   </si>
 </sst>
 </file>
@@ -241,12 +422,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,4 +1052,262 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F45D7E-DE8A-4050-BFDA-DD51E35CA441}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="135" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8786407-E05E-4B9D-8690-5D077E9E5DC2}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>